<commit_message>
updated data model per testing scrnaseq
</commit_message>
<xml_diff>
--- a/RFC Tables/EL RFC Metabolomics Human Data Model.xlsx
+++ b/RFC Tables/EL RFC Metabolomics Human Data Model.xlsx
@@ -1251,7 +1251,7 @@
 ProcessingBatchSizeUnit = other</t>
   </si>
   <si>
-    <t>dataFile</t>
+    <t>f</t>
   </si>
   <si>
     <t>The data file provides the name of the raw file generated by the instrument. The data files can be instrument raw files but also converted peak lists such as mzML, MGF or result files like mzIdentML.</t>
@@ -5717,7 +5717,7 @@
       <c r="AD67" s="30"/>
     </row>
     <row r="68">
-      <c r="A68" s="42" t="s">
+      <c r="A68" s="41" t="s">
         <v>211</v>
       </c>
       <c r="B68" s="42" t="s">

</xml_diff>